<commit_message>
csv-files for most popular tweets
</commit_message>
<xml_diff>
--- a/analysis/content_analysis/topics_quarters.xlsx
+++ b/analysis/content_analysis/topics_quarters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roth_\Uni\3.Semester_WS2021\Forschungsseminar\GitHub\UR_MI_FS_WS_20_21_Group_G\analysis\content_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73957994-9FEB-4F70-BADD-35AFE02CE822}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032D4E62-092E-4A61-A7E7-19842B01B1CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{373180F9-22F9-4A16-8269-7934239A5C4D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>(4, '0.011*"tb" + 0.008*"zeit" + 0.008*"corona" + 0.005*"jed" + 0.005*"draußen" + 0.005*"deutschland"')</t>
   </si>
@@ -54,21 +54,6 @@
     <t>Quartal 2</t>
   </si>
   <si>
-    <t>(0, '0.013*"amp" + 0.010*"jed" + 0.006*"bundesregierung" + 0.006*"tag" + 0.005*"deutschland" + 0.005*"bundestag"')</t>
-  </si>
-  <si>
-    <t>(1, '0.014*"corona" + 0.014*"amp" + 0.009*"frage" + 0.007*"jahr" + 0.006*"coronakrise" + 0.006*"zeit"')</t>
-  </si>
-  <si>
-    <t>(2, '0.010*"amp" + 0.009*"mensch" + 0.009*"corona" + 0.007*"jahr" + 0.005*"land" + 0.004*"frau"')</t>
-  </si>
-  <si>
-    <t>(3, '0.012*"deutschland" + 0.007*"afd" + 0.006*"is" + 0.005*"spd" + 0.005*"jahr" + 0.004*"trump"')</t>
-  </si>
-  <si>
-    <t>(4, '0.011*"amp" + 0.008*"berlin" + 0.007*"bundestag" + 0.006*"afd" + 0.006*"zeit" + 0.005*"mensch"')</t>
-  </si>
-  <si>
     <t>Quartal 3</t>
   </si>
   <si>
@@ -132,13 +117,40 @@
     <t>Corona in Deutschland</t>
   </si>
   <si>
-    <t>Lockdown?</t>
-  </si>
-  <si>
     <t>&gt; wenig corona</t>
   </si>
   <si>
     <t>&gt; Paar Themen die rausstechen, Corona zieht sich durch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(0, '0.012*"kind" + 0.007*"corona" + 0.007*"berlin" + 0.007*"schule" + 0.006*"frage" + 0.005*"afd"'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1, '0.013*"deutschland" + 0.012*"afd" + 0.008*"jahr" + 0.006*"polizei" + 0.006*"amp" + 0.005*"klaren"'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2, '0.010*"bundestag" + 0.010*"amp" + 0.009*"corona" + 0.006*"jahr" + 0.006*"mensch" + 0.006*"woche"'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3, '0.008*"is" + 0.006*"on" + 0.005*"i" + 0.005*"we" + 0.005*"rassismus" + 0.005*"trump"'), </t>
+  </si>
+  <si>
+    <t>(4, '0.022*"amp" + 0.010*"mensch" + 0.010*"coronakrise" + 0.009*"corona" + 0.008*"zeit" + 0.007*"krise"')]</t>
+  </si>
+  <si>
+    <t>Schuschließungen</t>
+  </si>
+  <si>
+    <t>Coronadebatten im Bundestag</t>
+  </si>
+  <si>
+    <t>Trump und Rassismus</t>
+  </si>
+  <si>
+    <t>Coronakrise</t>
+  </si>
+  <si>
+    <t>Lockdown weniger Kommuniziert</t>
   </si>
 </sst>
 </file>
@@ -502,24 +514,25 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="100" customWidth="1"/>
     <col min="2" max="2" width="37.21875" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -527,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -545,7 +558,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -560,113 +573,125 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
         <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>